<commit_message>
Fixed formatting and typos
</commit_message>
<xml_diff>
--- a/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
+++ b/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CIS195-CourseMaterials/LabStarters/Lab02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CIS195-CourseMaterials\LabStarters\Lab02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA6BBA-4AE2-DA43-A1A6-210BFB4B1598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA4FB81-C95F-45E9-889B-414160436216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15900" yWindow="7660" windowWidth="15660" windowHeight="17280" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="43500" yWindow="-4260" windowWidth="10200" windowHeight="16680" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>Elements used:</t>
   </si>
@@ -86,6 +95,9 @@
   </si>
   <si>
     <t>Correct code format</t>
+  </si>
+  <si>
+    <t>Horizontal rule</t>
   </si>
 </sst>
 </file>
@@ -470,17 +482,17 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,7 +503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -502,7 +514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -513,7 +525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -524,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -535,7 +547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -546,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -557,7 +569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -568,7 +580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -579,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -592,12 +604,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -608,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -619,7 +631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -630,7 +642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -641,7 +653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -652,7 +664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -663,7 +675,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -674,7 +686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -685,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -708,20 +720,20 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -732,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -743,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -754,7 +766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -765,7 +777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -776,9 +788,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -787,7 +799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -798,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -809,7 +821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -820,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -833,12 +845,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -849,7 +861,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -860,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -871,7 +883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -882,7 +894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -893,7 +905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -904,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -915,7 +927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -926,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Updates to lab instructions
They now contain links to the rubrics
</commit_message>
<xml_diff>
--- a/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
+++ b/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
@@ -1,41 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CIS195-CourseMaterials\LabStarters\Lab02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CIS195-CourseMaterials/LabStarters/Lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA4FB81-C95F-45E9-889B-414160436216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1796DD0-6B89-CA48-BC75-5F807ADD6A1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43500" yWindow="-4260" windowWidth="10200" windowHeight="16680" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="39940" yWindow="500" windowWidth="11260" windowHeight="17020" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>Elements used:</t>
   </si>
@@ -98,6 +89,9 @@
   </si>
   <si>
     <t>Horizontal rule</t>
+  </si>
+  <si>
+    <t>Points</t>
   </si>
 </sst>
 </file>
@@ -478,120 +472,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -599,105 +570,82 @@
         <f>SUM(B3:B10)</f>
         <v>20</v>
       </c>
-      <c r="C11" s="3">
-        <f>SUM(C3:C10)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="2">
         <v>5</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2">
         <v>2</v>
       </c>
-      <c r="C20" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -705,10 +653,7 @@
         <f>SUM(B14:B21)</f>
         <v>30</v>
       </c>
-      <c r="C22" s="3">
-        <f>SUM(C14:C21)</f>
-        <v>30</v>
-      </c>
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -719,21 +664,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.69921875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,7 +689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -755,7 +700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -766,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -777,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -788,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -799,7 +744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -810,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -821,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -832,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -845,12 +790,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -861,7 +806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -872,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -883,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -894,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -905,7 +850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -916,7 +861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -927,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -938,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Significant revision to lab instructions
Update to notes
</commit_message>
<xml_diff>
--- a/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
+++ b/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27327092-0FE3-464C-BCC5-21BF948DB7CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16158670-3270-1A48-BA92-97B6C768A3BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12840" yWindow="620" windowWidth="15960" windowHeight="15580" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>Correct syntax</t>
   </si>
   <si>
-    <t>Correct code format</t>
-  </si>
-  <si>
     <t>Horizontal rule</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>Best practices</t>
+  </si>
+  <si>
+    <t>Best Practices</t>
   </si>
 </sst>
 </file>
@@ -160,12 +160,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +504,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -563,7 +566,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -571,7 +574,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3">
         <f>SUM(B3:B10)</f>
@@ -588,7 +591,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -641,7 +644,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
@@ -649,7 +652,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <f>SUM(B14:B21)</f>
@@ -659,7 +662,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <f>B11+B22</f>
@@ -673,10 +676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -684,7 +687,7 @@
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -749,7 +752,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -782,7 +785,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
@@ -793,7 +796,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3">
         <f>SUM(B3:B10)</f>
@@ -888,7 +891,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
@@ -899,7 +902,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3">
         <f>SUM(B14:B21)</f>

</xml_diff>

<commit_message>
Updated grading rubrics, clarified instructions
</commit_message>
<xml_diff>
--- a/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
+++ b/LabStarters/Lab02/Lab2Rubric-CS195.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16158670-3270-1A48-BA92-97B6C768A3BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD0EB82E-FAF0-A142-9FEA-71A42C8AD0A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="620" windowWidth="15960" windowHeight="15580" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="8440" yWindow="620" windowWidth="15960" windowHeight="15580" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -483,15 +483,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -661,10 +662,15 @@
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B24" s="1">
         <f>B11+B22</f>
         <v>40</v>
       </c>
@@ -678,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>